<commit_message>
Update schedule file: Y5_B2425_Pediatrics_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y5_B2425_Pediatrics_schedule.xlsx
+++ b/modules_schedules/Y5_B2425_Pediatrics_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,7 +560,7 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>PED-B2-1</t>
+          <t>PED-B2-2</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
@@ -570,12 +570,12 @@
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E3" s="7" t="inlineStr">
         <is>
-          <t>31/08/2025</t>
+          <t>30/08/2025</t>
         </is>
       </c>
       <c r="F3" s="8" t="inlineStr">
@@ -584,6 +584,146 @@
         </is>
       </c>
       <c r="G3" s="9" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>PED-B2-3</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>pediatrics</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>30/08/2025</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>PED-B2-4</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>pediatrics</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>30/08/2025</t>
+        </is>
+      </c>
+      <c r="F5" s="8" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G5" s="9" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>PED-B2-5</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>pediatrics</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>30/08/2025</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>PED-B2-6</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>pediatrics</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="inlineStr">
+        <is>
+          <t>30/08/2025</t>
+        </is>
+      </c>
+      <c r="F7" s="8" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G7" s="9" t="n">
         <v>240</v>
       </c>
     </row>

</xml_diff>